<commit_message>
chore: publish conditionlist IG 1.0.1
</commit_message>
<xml_diff>
--- a/ig/conditionlist/StructureDefinition-medcom-conditionlist-bundle.xlsx
+++ b/ig/conditionlist/StructureDefinition-medcom-conditionlist-bundle.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0</t>
+    <t>1.0.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-11-15T10:26:02+01:00</t>
+    <t>2025-05-12T13:35:50+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1313,17 +1313,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="70.12890625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="38.1796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="32.3984375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="4" max="4" width="20.859375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="5" max="5" width="5.90234375" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="4.69921875" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="5.07421875" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="14.625" customWidth="true" bestFit="true"/>
-    <col min="9" max="9" width="11.98828125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="61.1171875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="33.44140625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="28.0390625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="4" max="4" width="18.19140625" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="5" max="5" width="5.80859375" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="4.23828125" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="4.65625" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.953125" customWidth="true" bestFit="true"/>
+    <col min="9" max="9" width="11.3671875" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="98.55859375" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="85.1484375" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -1332,26 +1332,26 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="8.84375" customWidth="true" bestFit="true"/>
-    <col min="21" max="21" width="15.71484375" customWidth="true" bestFit="true"/>
-    <col min="22" max="22" width="16.08984375" customWidth="true" bestFit="true"/>
-    <col min="23" max="23" width="17.078125" customWidth="true" bestFit="true"/>
-    <col min="24" max="24" width="16.3125" customWidth="true" bestFit="true"/>
-    <col min="25" max="25" width="163.2734375" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="49.55078125" customWidth="true" bestFit="true"/>
-    <col min="27" max="27" width="5.69140625" customWidth="true" bestFit="true"/>
-    <col min="28" max="28" width="19.73046875" customWidth="true" bestFit="true"/>
-    <col min="29" max="29" width="31.609375" customWidth="true" bestFit="true"/>
-    <col min="30" max="30" width="14.98828125" customWidth="true" bestFit="true"/>
-    <col min="31" max="31" width="12.3046875" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="32" max="32" width="34.5859375" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="33" max="33" width="9.5" customWidth="true" bestFit="true" hidden="true"/>
-    <col min="34" max="34" width="9.87890625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="8.53515625" customWidth="true" bestFit="true"/>
+    <col min="21" max="21" width="14.72265625" customWidth="true" bestFit="true"/>
+    <col min="22" max="22" width="15.13671875" customWidth="true" bestFit="true"/>
+    <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
+    <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
+    <col min="25" max="25" width="144.1953125" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="42.01953125" customWidth="true" bestFit="true"/>
+    <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
+    <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
+    <col min="29" max="29" width="28.21875" customWidth="true" bestFit="true"/>
+    <col min="30" max="30" width="14.7578125" customWidth="true" bestFit="true"/>
+    <col min="31" max="31" width="12.359375" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="32" max="32" width="29.98828125" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="33" max="33" width="9.046875" customWidth="true" bestFit="true" hidden="true"/>
+    <col min="34" max="34" width="9.46484375" customWidth="true" bestFit="true"/>
     <col min="35" max="35" width="100.703125" customWidth="true"/>
-    <col min="37" max="37" width="25.01171875" customWidth="true" bestFit="true"/>
-    <col min="38" max="38" width="64.8125" customWidth="true" bestFit="true"/>
-    <col min="39" max="39" width="41.43359375" customWidth="true" bestFit="true"/>
-    <col min="40" max="40" width="32.84375" customWidth="true" bestFit="true"/>
+    <col min="37" max="37" width="24.1328125" customWidth="true" bestFit="true"/>
+    <col min="38" max="38" width="57.64453125" customWidth="true" bestFit="true"/>
+    <col min="39" max="39" width="36.84375" customWidth="true" bestFit="true"/>
+    <col min="40" max="40" width="31.65234375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">

</xml_diff>